<commit_message>
Added week 6 and 8 evidence
</commit_message>
<xml_diff>
--- a/Week_05/Money Cash Board Constraints Plan.xlsx
+++ b/Week_05/Money Cash Board Constraints Plan.xlsx
@@ -59,43 +59,44 @@
     <t>Budgets</t>
   </si>
   <si>
-    <t>Needs further development to ensure all types of users are catered for</t>
-  </si>
-  <si>
-    <t>Does not provide enough options for the user to effectively manage their budget.</t>
-  </si>
-  <si>
-    <t>Database neds adjusting to include a budget table, that could then be manipulated and sorted by a model.</t>
-  </si>
-  <si>
-    <t>Lacks usability identified during design phase as important, from user needs. Cannot be used across different platfrom types, due to not being usable on small screens like phones and tablets.</t>
-  </si>
-  <si>
-    <t>Uasability can impacted by lack of portability.
-Not accessible to all user types.</t>
-  </si>
-  <si>
-    <t>Website is designed on a tabular layout which has ben made accessible for screen readers. Navigation is provided by large accessible buttons, and mouse clicks are reduced to a minimum. 
-Further work required on portability aspects.</t>
-  </si>
-  <si>
     <t>No budget allocated for the project by CodeClan</t>
   </si>
   <si>
     <t>Constarint not applicable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.5 days development time for MVP and extensions was allocated by CodeClan. Schedule very tight. </t>
   </si>
   <si>
     <t>Produced good workable plan in 0.5 days which allowed the build to progress for 4 full days.
 Maximised time on-site to gain fullest possible support from instructors and Cohort members.</t>
   </si>
   <si>
-    <t>No transactions, but storage may be an issue in the future depending on the volume of users.</t>
-  </si>
-  <si>
-    <t>Database would have to be expanded to accommodate.</t>
+    <t>Lacks usability identified during design phase as important, from user needs. Cannot be used across different platfrom types, due to not being usable on small screens like phones and tablets. This will have an impact on the potential market and reduce take-up.</t>
+  </si>
+  <si>
+    <t>Does not provide enough options for the user to effectively manage their budget. Users will prefer to use competitor product which includes this functionality.</t>
+  </si>
+  <si>
+    <t>No transactions, but storage may be an issue in the future depending on the volume of users. Not considered to be a major significant business risk at this point, but will become an issue when userbase increases.</t>
+  </si>
+  <si>
+    <t>Uasability can impacted by lack of portability.
+Not accessible to all user types, which will reduce appeal, and have an impact on the volume of users.</t>
+  </si>
+  <si>
+    <t>4.5 days development time for MVP and extensions was allocated by CodeClan. Schedule very tight. 
+Basic product not visually appealing which will affect marketability.</t>
+  </si>
+  <si>
+    <t>Needs further development to ensure all types of users are catered for. Different media types can be easily catered for using Flexbox &amp; media queries in CSS.</t>
+  </si>
+  <si>
+    <t>Database neds adjusting to include a budget table that could then be manipulated and sorted by a model.</t>
+  </si>
+  <si>
+    <t>Database would have to be expanded to accommodate. This could be achieved by changing the Transactions table from INT2 to INT8.</t>
+  </si>
+  <si>
+    <t>Website is designed on a tabular layout which has ben made accessible for screen readers. Navigation is provided by large accessible buttons, and mouse clicks are reduced to a minimum. 
+Further work required on portability aspects, as per Hardware &amp; Software constraint above.</t>
   </si>
 </sst>
 </file>
@@ -253,19 +254,55 @@
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -275,42 +312,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,7 +593,7 @@
   <dimension ref="B3:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,141 +604,139 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="9" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="14"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="2:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="1" t="s">
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="2:8" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="2:8" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="6" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="1" t="s">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="2:8" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="2:8" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="2:8" ht="83" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="2:8" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="3"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="G3:H4"/>
-    <mergeCell ref="D3:F4"/>
     <mergeCell ref="B3:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
@@ -745,14 +744,11 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G9:H9"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="G3:H4"/>
+    <mergeCell ref="D3:F4"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:F10"/>
@@ -763,6 +759,11 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>